<commit_message>
- Agenda Vehicular: Campo Destino - Nuevo Evento: Vehiculo Agendado - SpeedTickets: Chofer x Reservado - Reporte Km Diarios: Nuevos campos para EDESUR. Link al Resumen de Recorrido -
</commit_message>
<xml_diff>
--- a/Logictracker/Logictracker/src/Web/Logictracker/Logictracker.Web/ExcelTemplate/Logictracker/KilometrosDiarios.xlsx
+++ b/Logictracker/Logictracker/src/Web/Logictracker/Logictracker.Web/ExcelTemplate/Logictracker/KilometrosDiarios.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\Logictracker\Logictracker\Logictracker\src\Web\Logictracker\Logictracker.Web\ExcelTemplate\Logictracker\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="240" yWindow="150" windowWidth="14115" windowHeight="5700"/>
   </bookViews>
@@ -10,34 +15,62 @@
     <sheet name="Informe" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Informe!$A$7:$D$7</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Informe!$A$7:$K$7</definedName>
+    <definedName name="HS_DETENIDO">Informe!$F$7</definedName>
+    <definedName name="HS_DETENIDO_BASE">Informe!$I$7</definedName>
+    <definedName name="HS_DETENIDO_CON_TAREA">Informe!$J$7</definedName>
+    <definedName name="HS_DETENIDO_SIN_TAREA">Informe!$K$7</definedName>
+    <definedName name="HS_DETENIDO_TALLER">Informe!$H$7</definedName>
+    <definedName name="HS_MARCHA">Informe!$D$7</definedName>
+    <definedName name="HS_MOVIMIENTO">Informe!$E$7</definedName>
+    <definedName name="HS_SIN_REPORTAR">Informe!$G$7</definedName>
+    <definedName name="KM_EN_RUTA">Informe!$C$7</definedName>
+    <definedName name="KM_TOTALES">Informe!$B$7</definedName>
+    <definedName name="PATENTE">Informe!$A$7</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="0">Informe!$A:$B</definedName>
-    <definedName name="FECHA">Informe!$B$7</definedName>
-    <definedName name="KM_EN_RUTA">Informe!$D$7</definedName>
-    <definedName name="KM_TOTALES">Informe!$C$7</definedName>
-    <definedName name="PARENTI03">Informe!$A$7</definedName>
-    <definedName name="Titulo">Informe!$C$1</definedName>
+    <definedName name="Titulo">Informe!$D$1</definedName>
   </definedNames>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Funciones</t>
-  </si>
-  <si>
-    <t>Vehículo</t>
   </si>
   <si>
     <t>Km Totales</t>
   </si>
   <si>
-    <t>Fecha</t>
+    <t>Km en Ruta</t>
   </si>
   <si>
-    <t>Km en Ruta</t>
+    <t>Patente</t>
+  </si>
+  <si>
+    <t>Horas en Marcha</t>
+  </si>
+  <si>
+    <t>Horas en Movimiento</t>
+  </si>
+  <si>
+    <t>Horas Detenido</t>
+  </si>
+  <si>
+    <t>Horas Sin Reportar</t>
+  </si>
+  <si>
+    <t>Horas Detenido en Taller</t>
+  </si>
+  <si>
+    <t>Horas Detenido en Base</t>
+  </si>
+  <si>
+    <t>Horas Detenido con Tarea</t>
+  </si>
+  <si>
+    <t>Horas Detenido sin Tarea</t>
   </si>
 </sst>
 </file>
@@ -574,48 +607,48 @@
     <xf numFmtId="0" fontId="17" fillId="33" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="42">
-    <cellStyle name="20% - Énfasis1" xfId="19" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="20% - Énfasis2" xfId="23" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="20% - Énfasis3" xfId="27" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="20% - Énfasis4" xfId="31" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="20% - Énfasis5" xfId="35" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="20% - Énfasis6" xfId="39" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="40% - Énfasis1" xfId="20" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="40% - Énfasis2" xfId="24" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="40% - Énfasis3" xfId="28" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="40% - Énfasis4" xfId="32" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="40% - Énfasis5" xfId="36" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="40% - Énfasis6" xfId="40" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="60% - Énfasis1" xfId="21" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="60% - Énfasis2" xfId="25" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="60% - Énfasis3" xfId="29" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="60% - Énfasis4" xfId="33" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="60% - Énfasis5" xfId="37" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="60% - Énfasis6" xfId="41" builtinId="52" customBuiltin="1"/>
-    <cellStyle name="Buena" xfId="6" builtinId="26" customBuiltin="1"/>
-    <cellStyle name="Cálculo" xfId="11" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="Celda de comprobación" xfId="13" builtinId="23" customBuiltin="1"/>
-    <cellStyle name="Celda vinculada" xfId="12" builtinId="24" customBuiltin="1"/>
-    <cellStyle name="Encabezado 4" xfId="5" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="Énfasis1" xfId="18" builtinId="29" customBuiltin="1"/>
-    <cellStyle name="Énfasis2" xfId="22" builtinId="33" customBuiltin="1"/>
-    <cellStyle name="Énfasis3" xfId="26" builtinId="37" customBuiltin="1"/>
-    <cellStyle name="Énfasis4" xfId="30" builtinId="41" customBuiltin="1"/>
-    <cellStyle name="Énfasis5" xfId="34" builtinId="45" customBuiltin="1"/>
-    <cellStyle name="Énfasis6" xfId="38" builtinId="49" customBuiltin="1"/>
-    <cellStyle name="Entrada" xfId="9" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="Incorrecto" xfId="7" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40% - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60% - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60% - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60% - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60% - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60% - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="Accent1" xfId="18" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="Accent2" xfId="22" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="Accent3" xfId="26" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="Accent4" xfId="30" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="Accent5" xfId="34" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="Accent6" xfId="38" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Notas" xfId="15" builtinId="10" customBuiltin="1"/>
-    <cellStyle name="Salida" xfId="10" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="Texto de advertencia" xfId="14" builtinId="11" customBuiltin="1"/>
-    <cellStyle name="Texto explicativo" xfId="16" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="Título" xfId="1" builtinId="15" customBuiltin="1"/>
-    <cellStyle name="Título 1" xfId="2" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Título 2" xfId="3" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Título 3" xfId="4" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
+    <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -627,6 +660,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -642,8 +678,8 @@
       <xdr:rowOff>47625</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>1038224</xdr:colOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>866774</xdr:colOff>
       <xdr:row>4</xdr:row>
       <xdr:rowOff>87915</xdr:rowOff>
     </xdr:to>
@@ -682,7 +718,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -724,7 +760,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -759,7 +795,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -971,48 +1007,89 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:K8"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.5703125" style="2" customWidth="1"/>
-    <col min="2" max="2" width="27" customWidth="1"/>
-    <col min="3" max="3" width="15.5703125" customWidth="1"/>
-    <col min="4" max="4" width="17.42578125" customWidth="1"/>
+    <col min="1" max="1" width="14.140625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="13" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="25.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="24.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="26.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="25.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="31.5" x14ac:dyDescent="0.5">
-      <c r="C1" s="4" t="s">
+    <row r="1" spans="1:11" ht="31.5" x14ac:dyDescent="0.5">
+      <c r="D1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="1"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="4"/>
+      <c r="I1" s="4"/>
+      <c r="J1" s="4"/>
+      <c r="K1" s="4"/>
     </row>
-    <row r="2" spans="1:4" ht="4.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" ht="4.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
+      <c r="K2" s="1"/>
     </row>
-    <row r="3" spans="1:4" ht="4.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" ht="4.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+      <c r="J3" s="1"/>
+      <c r="K3" s="1"/>
     </row>
-    <row r="4" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+      <c r="J4" s="1"/>
+      <c r="K4" s="1"/>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+      <c r="J5" s="1"/>
+      <c r="K5" s="1"/>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C7" s="5" t="s">
         <v>2</v>
@@ -1020,15 +1097,43 @@
       <c r="D7" s="5" t="s">
         <v>4</v>
       </c>
+      <c r="E7" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="G7" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="H7" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="I7" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="J7" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="K7" s="5" t="s">
+        <v>11</v>
+      </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="3"/>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
+      <c r="H8" s="3"/>
+      <c r="I8" s="3"/>
+      <c r="J8" s="3"/>
+      <c r="K8" s="3"/>
     </row>
   </sheetData>
-  <autoFilter ref="A7:D7"/>
+  <autoFilter ref="A7:K7"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="92" fitToHeight="0" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>

</xml_diff>